<commit_message>
Cosas, nota: RFC 10 disfuncional.
</commit_message>
<xml_diff>
--- a/sistrans/Docs/RotondAndes Documentacion Modelo Relacional.xlsx
+++ b/sistrans/Docs/RotondAndes Documentacion Modelo Relacional.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\SkyDrive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\SMSBayern\sistrans\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="218">
   <si>
     <t>Nombre</t>
   </si>
@@ -101,9 +101,6 @@
     <t>MESA</t>
   </si>
   <si>
-    <t>Tabla que contiene a los clientes frecuentes</t>
-  </si>
-  <si>
     <t>PASSWORD</t>
   </si>
   <si>
@@ -144,12 +141,6 @@
   </si>
   <si>
     <t>Varchar2(40 Byte)</t>
-  </si>
-  <si>
-    <t>Contraseña del Cliente Frecuente.</t>
-  </si>
-  <si>
-    <t>ID con la que se identifica el Cliente</t>
   </si>
   <si>
     <t>Descripción en español.</t>
@@ -330,23 +321,10 @@
 a cierto Producto (Producto 1).</t>
   </si>
   <si>
-    <t>REPRESENTA</t>
-  </si>
-  <si>
     <t>ID_PRODUCTO1, ID_PRODUCTO2</t>
   </si>
   <si>
     <t>ID_CLIENTEFRECUENTE, ID_PRODUCTO</t>
-  </si>
-  <si>
-    <t>Tabla que contiene la información de la relación de qué Representante representa a qué restaurante.
-a cierto Producto (Producto 1).</t>
-  </si>
-  <si>
-    <t>ID_REPRESENTANTE</t>
-  </si>
-  <si>
-    <t>ID_RESTAURANTE, ID_REPRESENTANTE</t>
   </si>
   <si>
     <t>REPRESENTANTES</t>
@@ -396,18 +374,9 @@
     <t>ID de la Zona asignada a este Restaurante.</t>
   </si>
   <si>
-    <t>TIPOPRODUCTO</t>
-  </si>
-  <si>
     <t>ID_PROD</t>
   </si>
   <si>
-    <t>ID del Tipo de Producto asociado al Producto.</t>
-  </si>
-  <si>
-    <t>ID del Producto asociado a un Tipo.</t>
-  </si>
-  <si>
     <t>ID_PROD, ID_TIPO</t>
   </si>
   <si>
@@ -448,9 +417,6 @@
   </si>
   <si>
     <t>Booleano que indica si es espacio Abierto.</t>
-  </si>
-  <si>
-    <t>NN, SA, NC, PK, FK_CLIENTEFR</t>
   </si>
   <si>
     <t>NN, UA, FK, PK, FK_CONDICIONDELAZONA</t>
@@ -572,12 +538,6 @@
     <t>Nombre del Producto.</t>
   </si>
   <si>
-    <t>NN, UA, ND, CK, PK, FK_RESTAURANTES</t>
-  </si>
-  <si>
-    <t>NN, UA, CK, PK, FK_REPRESENTANTES</t>
-  </si>
-  <si>
     <t>PAGINA_WEB</t>
   </si>
   <si>
@@ -593,9 +553,6 @@
     <t>NN, UA, FK_ZONAS</t>
   </si>
   <si>
-    <t>NN, UA, PK, FK_TIPOS</t>
-  </si>
-  <si>
     <t>NN, ND, UA</t>
   </si>
   <si>
@@ -644,10 +601,91 @@
     <t>CONDICIONESTECNICAS</t>
   </si>
   <si>
-    <t>CLIENTESFRECUENTES</t>
-  </si>
-  <si>
     <t>CLIENTES</t>
+  </si>
+  <si>
+    <t>MENUS_PEDIDOS</t>
+  </si>
+  <si>
+    <t>Tabla que contiene los Pedidos de un Menú</t>
+  </si>
+  <si>
+    <t>IDMENU</t>
+  </si>
+  <si>
+    <t>IDORDEN</t>
+  </si>
+  <si>
+    <t>ID del Menú Pedido.</t>
+  </si>
+  <si>
+    <t>ID de la Orden Pedida</t>
+  </si>
+  <si>
+    <t>NN, UA, FK_MENUS_PEDIDOS_MENUS</t>
+  </si>
+  <si>
+    <t>NN, UA, FK_MENUS_PEDIDOS_ORDENES</t>
+  </si>
+  <si>
+    <t>REGISTROVENTAS</t>
+  </si>
+  <si>
+    <t>Tabla que contiene la información del registro de ventas de una semana</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>IDPRODUCTOMASVENDIDO</t>
+  </si>
+  <si>
+    <t>IDPRODUCTOMENOSVENDIDO</t>
+  </si>
+  <si>
+    <t>IDRESTAURNTEMASFREUENTADO</t>
+  </si>
+  <si>
+    <t>IDRESTAURANTEMENOSFRECUENTADO</t>
+  </si>
+  <si>
+    <t>Día de la semana</t>
+  </si>
+  <si>
+    <t>ID producto más vendido.</t>
+  </si>
+  <si>
+    <t>ID producto menos vendido.</t>
+  </si>
+  <si>
+    <t>ID restaurante mas frecuentado.</t>
+  </si>
+  <si>
+    <t>ID restaurante menos frecuentado</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>USUARIOS</t>
+  </si>
+  <si>
+    <t>Tabla que contiene la información básica de los Usuarios</t>
+  </si>
+  <si>
+    <t>ROL</t>
+  </si>
+  <si>
+    <t>Varchar2  (255 BYTE)</t>
+  </si>
+  <si>
+    <t>ID del usuario.</t>
+  </si>
+  <si>
+    <t>Contraseña del Usuario</t>
+  </si>
+  <si>
+    <t>PK, SA</t>
   </si>
 </sst>
 </file>
@@ -981,7 +1019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1033,24 +1071,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1069,6 +1089,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1076,6 +1114,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1096,16 +1146,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1388,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E175"/>
+  <dimension ref="B1:E197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="I153" sqref="I153"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,21 +1450,21 @@
       <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
@@ -1495,97 +1539,61 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="45" t="s">
-        <v>203</v>
-      </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="46"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="51"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="44"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>21</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="48"/>
       <c r="E12" s="49"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>140</v>
-      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>15</v>
-      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="45" t="s">
-        <v>202</v>
-      </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="46"/>
+      <c r="C17" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="50"/>
+      <c r="E17" s="51"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="44"/>
+      <c r="C18" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="46"/>
     </row>
     <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
@@ -1619,7 +1627,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>18</v>
@@ -1630,10 +1638,10 @@
         <v>22</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>15</v>
@@ -1644,28 +1652,28 @@
       <c r="B24" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="45" t="s">
-        <v>201</v>
-      </c>
-      <c r="D24" s="45"/>
-      <c r="E24" s="46"/>
+      <c r="C24" s="50" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24" s="50"/>
+      <c r="E24" s="51"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="43"/>
-      <c r="E25" s="44"/>
+      <c r="C25" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="45"/>
+      <c r="E25" s="46"/>
     </row>
     <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="48"/>
       <c r="E26" s="49"/>
@@ -1686,30 +1694,30 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1717,31 +1725,31 @@
       <c r="B32" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="45" t="s">
-        <v>200</v>
-      </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="46"/>
+      <c r="C32" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" s="50"/>
+      <c r="E32" s="51"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="43"/>
-      <c r="E33" s="44"/>
+      <c r="C33" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="45"/>
+      <c r="E33" s="46"/>
     </row>
     <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="42"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="53"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="22" t="s">
@@ -1765,7 +1773,7 @@
         <v>12</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>8</v>
@@ -1776,24 +1784,24 @@
         <v>22</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>7</v>
@@ -1801,13 +1809,13 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>7</v>
@@ -1815,16 +1823,16 @@
     </row>
     <row r="40" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="28" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C40" s="29" t="s">
         <v>12</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1832,31 +1840,31 @@
       <c r="B42" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="45" t="s">
-        <v>199</v>
-      </c>
-      <c r="D42" s="45"/>
-      <c r="E42" s="46"/>
+      <c r="C42" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="D42" s="50"/>
+      <c r="E42" s="51"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="43"/>
-      <c r="E43" s="44"/>
+      <c r="C43" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="45"/>
+      <c r="E43" s="46"/>
     </row>
     <row r="44" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="41"/>
-      <c r="E44" s="42"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="53"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="22" t="s">
@@ -1880,38 +1888,38 @@
         <v>12</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="17" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1924,28 +1932,28 @@
       <c r="B50" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="50" t="s">
-        <v>198</v>
-      </c>
-      <c r="D50" s="51"/>
-      <c r="E50" s="52"/>
+      <c r="C50" s="54" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50" s="55"/>
+      <c r="E50" s="56"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="D51" s="54"/>
-      <c r="E51" s="55"/>
+      <c r="C51" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="58"/>
+      <c r="E51" s="59"/>
     </row>
     <row r="52" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="25" t="s">
         <v>2</v>
       </c>
       <c r="C52" s="47" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D52" s="48"/>
       <c r="E52" s="49"/>
@@ -1966,44 +1974,44 @@
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C54" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="19" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C56" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2011,31 +2019,31 @@
       <c r="B58" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="45" t="s">
-        <v>197</v>
-      </c>
-      <c r="D58" s="45"/>
-      <c r="E58" s="46"/>
+      <c r="C58" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="D58" s="50"/>
+      <c r="E58" s="51"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="D59" s="43"/>
-      <c r="E59" s="44"/>
+      <c r="C59" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="45"/>
+      <c r="E59" s="46"/>
     </row>
     <row r="60" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="41" t="s">
+      <c r="C60" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D60" s="41"/>
-      <c r="E60" s="42"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="53"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="22" t="s">
@@ -2059,7 +2067,7 @@
         <v>12</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>8</v>
@@ -2070,80 +2078,80 @@
         <v>22</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C64" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E68" s="18" t="s">
         <v>10</v>
@@ -2151,16 +2159,16 @@
     </row>
     <row r="69" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C69" s="29" t="s">
         <v>12</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2168,31 +2176,31 @@
       <c r="B71" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C71" s="45" t="s">
-        <v>196</v>
-      </c>
-      <c r="D71" s="45"/>
-      <c r="E71" s="46"/>
+      <c r="C71" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="D71" s="50"/>
+      <c r="E71" s="51"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D72" s="43"/>
-      <c r="E72" s="44"/>
+      <c r="C72" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="D72" s="45"/>
+      <c r="E72" s="46"/>
     </row>
     <row r="73" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="41" t="s">
+      <c r="C73" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D73" s="41"/>
-      <c r="E73" s="42"/>
+      <c r="D73" s="52"/>
+      <c r="E73" s="53"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="22" t="s">
@@ -2216,7 +2224,7 @@
         <v>12</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E75" s="18" t="s">
         <v>8</v>
@@ -2224,619 +2232,619 @@
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="17" t="s">
-        <v>74</v>
+        <v>192</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="17" t="s">
-        <v>85</v>
+        <v>193</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>72</v>
+        <v>195</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C78" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D78" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E78" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="D79" s="50"/>
+      <c r="E79" s="51"/>
+    </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="15" t="s">
-        <v>0</v>
+      <c r="B80" s="16" t="s">
+        <v>1</v>
       </c>
       <c r="C80" s="45" t="s">
-        <v>195</v>
+        <v>66</v>
       </c>
       <c r="D80" s="45"/>
       <c r="E80" s="46"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C81" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D81" s="37"/>
-      <c r="E81" s="38"/>
-    </row>
-    <row r="82" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="25" t="s">
+    <row r="81" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C82" s="39" t="s">
+      <c r="C81" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D82" s="39"/>
-      <c r="E82" s="40"/>
+      <c r="D81" s="52"/>
+      <c r="E81" s="53"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82" s="24" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C83" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D83" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E83" s="24" t="s">
-        <v>5</v>
+      <c r="B83" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="17" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C84" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>82</v>
+        <v>176</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C86" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D86" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E86" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="D88" s="39"/>
+      <c r="E88" s="40"/>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D89" s="37"/>
+      <c r="E89" s="38"/>
+    </row>
+    <row r="90" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D90" s="35"/>
+      <c r="E90" s="36"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E91" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E92" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E93" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C85" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E85" s="18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C86" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D86" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="E86" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="C87" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="D87" s="27" t="s">
+      <c r="E94" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C95" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D95" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E95" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E96" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="C97" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D97" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="E97" s="30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C98" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E98" s="31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="E87" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C88" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D88" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="E88" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="C89" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D89" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="E89" s="30" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C90" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D90" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="E90" s="31" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C92" s="35" t="s">
+      <c r="D100" s="39"/>
+      <c r="E100" s="40"/>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="D92" s="35"/>
-      <c r="E92" s="36"/>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="D93" s="37"/>
-      <c r="E93" s="38"/>
-    </row>
-    <row r="94" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="25" t="s">
+      <c r="D101" s="37"/>
+      <c r="E101" s="38"/>
+    </row>
+    <row r="102" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C94" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="D94" s="39"/>
-      <c r="E94" s="40"/>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="22" t="s">
+      <c r="C102" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D102" s="35"/>
+      <c r="E102" s="36"/>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C95" s="23" t="s">
+      <c r="C103" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D95" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E95" s="24" t="s">
+      <c r="D103" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E103" s="24" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C96" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="E96" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C97" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D97" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="E97" s="21" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B99" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C99" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="D99" s="35"/>
-      <c r="E99" s="36"/>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="D100" s="37"/>
-      <c r="E100" s="38"/>
-    </row>
-    <row r="101" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C101" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="D101" s="39"/>
-      <c r="E101" s="40"/>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C102" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D102" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E102" s="24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B103" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C103" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D103" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="E103" s="18" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="17" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="C104" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="E104" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B105" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="C105" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D105" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="E105" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B106" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="C106" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D106" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="E106" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C107" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D107" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="E107" s="21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="33"/>
-      <c r="C108" s="33"/>
-      <c r="D108" s="33"/>
-      <c r="E108" s="33"/>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B109" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C105" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D105" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E105" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="15" t="s">
         <v>0</v>
       </c>
+      <c r="C107" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="D107" s="39"/>
+      <c r="E107" s="40"/>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="D108" s="37"/>
+      <c r="E108" s="38"/>
+    </row>
+    <row r="109" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="25" t="s">
+        <v>2</v>
+      </c>
       <c r="C109" s="35" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="D109" s="35"/>
       <c r="E109" s="36"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B110" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C110" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="D110" s="37"/>
-      <c r="E110" s="38"/>
-    </row>
-    <row r="111" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C111" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="D111" s="39"/>
-      <c r="E111" s="40"/>
+      <c r="B110" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C110" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D110" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E110" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C111" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D111" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E111" s="18" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B112" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C112" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D112" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E112" s="24" t="s">
-        <v>5</v>
+      <c r="B112" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D112" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E112" s="18" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D113" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E113" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E114" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C115" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D115" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="E115" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B116" s="33"/>
+      <c r="C116" s="33"/>
+      <c r="D116" s="33"/>
+      <c r="E116" s="33"/>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D117" s="39"/>
+      <c r="E117" s="40"/>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D118" s="37"/>
+      <c r="E118" s="38"/>
+    </row>
+    <row r="119" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B119" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C119" s="35" t="s">
         <v>21</v>
-      </c>
-      <c r="C113" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D113" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E113" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C114" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D114" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E114" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B115" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C115" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D115" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="E115" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="116" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B116" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="C116" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="D116" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="E116" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C117" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="D117" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="E117" s="21" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
-    </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C119" s="35" t="s">
-        <v>97</v>
       </c>
       <c r="D119" s="35"/>
       <c r="E119" s="36"/>
     </row>
     <row r="120" spans="2:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C120" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="D120" s="59"/>
-      <c r="E120" s="38"/>
-    </row>
-    <row r="121" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C121" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="D121" s="39"/>
-      <c r="E121" s="40"/>
+      <c r="B120" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C120" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D120" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E120" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B121" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D121" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E121" s="18" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B122" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C122" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D122" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E122" s="24" t="s">
-        <v>5</v>
+      <c r="B122" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D122" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E122" s="18" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" s="17" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>193</v>
+        <v>93</v>
       </c>
       <c r="E123" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B124" s="17" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D124" s="14" t="s">
-        <v>98</v>
+        <v>161</v>
+      </c>
+      <c r="D124" s="34" t="s">
+        <v>163</v>
       </c>
       <c r="E124" s="18" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
     </row>
     <row r="125" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="19" t="s">
-        <v>177</v>
+        <v>22</v>
       </c>
       <c r="C125" s="20" t="s">
-        <v>12</v>
+        <v>161</v>
       </c>
       <c r="D125" s="20" t="s">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="E125" s="21" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="126" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="126" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+    </row>
     <row r="127" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C127" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="D127" s="35"/>
-      <c r="E127" s="36"/>
+      <c r="C127" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D127" s="39"/>
+      <c r="E127" s="40"/>
     </row>
     <row r="128" spans="2:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C128" s="58" t="s">
-        <v>104</v>
-      </c>
-      <c r="D128" s="59"/>
+      <c r="C128" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D128" s="44"/>
       <c r="E128" s="38"/>
     </row>
     <row r="129" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C129" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="D129" s="39"/>
-      <c r="E129" s="40"/>
+      <c r="C129" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D129" s="35"/>
+      <c r="E129" s="36"/>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130" s="22" t="s">
@@ -2854,526 +2862,673 @@
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C131" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>62</v>
+        <v>179</v>
       </c>
       <c r="E131" s="18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="132" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C132" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D132" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="E132" s="21" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="133" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="134" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B132" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C132" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D132" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E132" s="18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B133" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C133" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D133" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E133" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="135" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C134" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="D134" s="35"/>
-      <c r="E134" s="36"/>
-    </row>
-    <row r="135" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C135" s="56" t="s">
-        <v>113</v>
-      </c>
-      <c r="D135" s="57"/>
-      <c r="E135" s="38"/>
-    </row>
-    <row r="136" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="25" t="s">
+      <c r="C135" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="D135" s="39"/>
+      <c r="E135" s="40"/>
+    </row>
+    <row r="136" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B136" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="D136" s="60"/>
+      <c r="E136" s="38"/>
+    </row>
+    <row r="137" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B137" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C136" s="39" t="s">
+      <c r="C137" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D136" s="39"/>
-      <c r="E136" s="40"/>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="22" t="s">
+      <c r="D137" s="35"/>
+      <c r="E137" s="36"/>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B138" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C137" s="23" t="s">
+      <c r="C138" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D137" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E137" s="24" t="s">
+      <c r="D138" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E138" s="24" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B138" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C138" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D138" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="E138" s="18" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B139" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C139" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D139" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E139" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B140" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C140" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D140" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E140" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B141" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C141" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D141" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E141" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="C142" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D142" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="E142" s="30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B143" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="C143" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D143" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="E143" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B146" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C146" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="D146" s="39"/>
+      <c r="E146" s="40"/>
+    </row>
+    <row r="147" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B147" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C147" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D147" s="42"/>
+      <c r="E147" s="38"/>
+    </row>
+    <row r="148" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B148" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C148" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D148" s="35"/>
+      <c r="E148" s="36"/>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B149" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C149" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D149" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E149" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B150" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C150" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D150" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E150" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B151" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C139" s="14" t="s">
+      <c r="C151" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D151" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E151" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B152" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C152" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D152" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E152" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="154" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B154" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C154" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="D154" s="39"/>
+      <c r="E154" s="40"/>
+    </row>
+    <row r="155" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B155" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C155" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="D155" s="44"/>
+      <c r="E155" s="38"/>
+    </row>
+    <row r="156" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C156" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D156" s="35"/>
+      <c r="E156" s="36"/>
+    </row>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B157" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C157" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D157" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E157" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B158" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C158" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D158" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E158" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B159" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C159" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D159" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E159" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="160" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C160" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D160" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E160" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="161" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C161" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D161" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="E161" s="30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B162" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C162" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D162" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E162" s="30" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="163" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B163" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C163" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D163" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="E163" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="172" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B172" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C172" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D172" s="39"/>
+      <c r="E172" s="40"/>
+    </row>
+    <row r="173" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B173" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C173" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="D173" s="44"/>
+      <c r="E173" s="38"/>
+    </row>
+    <row r="174" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B174" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C174" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="D139" s="14" t="s">
+      <c r="D174" s="35"/>
+      <c r="E174" s="36"/>
+    </row>
+    <row r="175" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B175" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C175" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D175" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E175" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B176" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C176" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D176" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E176" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B177" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C177" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="E139" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="140" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C140" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="D140" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="E140" s="21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="141" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="142" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="15" t="s">
+      <c r="D177" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E177" s="21" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="178" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B179" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C142" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="D142" s="35"/>
-      <c r="E142" s="36"/>
-    </row>
-    <row r="143" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C143" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D143" s="59"/>
-      <c r="E143" s="38"/>
-    </row>
-    <row r="144" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="25" t="s">
+      <c r="C179" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="D179" s="39"/>
+      <c r="E179" s="40"/>
+    </row>
+    <row r="180" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B180" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C180" s="61" t="s">
+        <v>212</v>
+      </c>
+      <c r="D180" s="61"/>
+      <c r="E180" s="38"/>
+    </row>
+    <row r="181" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B181" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C144" s="39" t="s">
+      <c r="C181" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D181" s="35"/>
+      <c r="E181" s="36"/>
+    </row>
+    <row r="182" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B182" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C182" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D182" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E182" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="183" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B183" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D144" s="39"/>
-      <c r="E144" s="40"/>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B145" s="22" t="s">
+      <c r="C183" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D183" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="E183" s="18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="184" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B184" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C184" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="D184" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E184" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="185" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B185" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="C185" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="D185" s="20"/>
+      <c r="E185" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="188" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="189" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B189" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C189" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="D189" s="39"/>
+      <c r="E189" s="40"/>
+    </row>
+    <row r="190" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B190" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C190" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="D190" s="44"/>
+      <c r="E190" s="38"/>
+    </row>
+    <row r="191" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B191" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C191" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D191" s="35"/>
+      <c r="E191" s="36"/>
+    </row>
+    <row r="192" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B192" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C145" s="23" t="s">
+      <c r="C192" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D145" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E145" s="24" t="s">
+      <c r="D192" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E192" s="24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B146" s="17" t="s">
+    <row r="193" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B193" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C146" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D146" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E146" s="18" t="s">
+      <c r="C193" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D193" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E193" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B147" s="17" t="s">
+    <row r="194" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B194" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C147" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D147" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="E147" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B148" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="C148" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="D148" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="E148" s="18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B149" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="C149" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D149" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="E149" s="30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="150" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B150" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C150" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D150" s="27" t="s">
+      <c r="C194" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D194" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E194" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B195" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E150" s="30" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="151" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="C151" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D151" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="E151" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="152" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="153" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C153" s="35" t="s">
+      <c r="C195" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D195" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E195" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="196" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B196" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D153" s="35"/>
-      <c r="E153" s="36"/>
-    </row>
-    <row r="154" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C154" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D154" s="59"/>
-      <c r="E154" s="38"/>
-    </row>
-    <row r="155" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C155" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D155" s="39"/>
-      <c r="E155" s="40"/>
-    </row>
-    <row r="156" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B156" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C156" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D156" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E156" s="24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B157" s="17" t="s">
+      <c r="C196" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D196" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E196" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="197" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B197" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C157" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D157" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="E157" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="158" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="C158" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D158" s="20" t="s">
+      <c r="C197" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E158" s="21" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="159" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="160" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C160" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="D160" s="35"/>
-      <c r="E160" s="36"/>
-    </row>
-    <row r="161" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C161" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D161" s="59"/>
-      <c r="E161" s="38"/>
-    </row>
-    <row r="162" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C162" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D162" s="39"/>
-      <c r="E162" s="40"/>
-    </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B163" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C163" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D163" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E163" s="24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B164" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C164" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D164" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="E164" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="165" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C165" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="D165" s="20" t="s">
+      <c r="D197" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="E165" s="21" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="166" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="167" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C167" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="D167" s="35"/>
-      <c r="E167" s="36"/>
-    </row>
-    <row r="168" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B168" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C168" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D168" s="59"/>
-      <c r="E168" s="38"/>
-    </row>
-    <row r="169" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C169" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D169" s="39"/>
-      <c r="E169" s="40"/>
-    </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B170" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C170" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D170" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E170" s="24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B171" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C171" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D171" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E171" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="172" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B172" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C172" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D172" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E172" s="18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B173" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="C173" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="D173" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="E173" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="174" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B174" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C174" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D174" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="E174" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="175" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C175" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="D175" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="E175" s="21" t="s">
-        <v>35</v>
+      <c r="E197" s="21" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C128:D128"/>
+  <mergeCells count="30">
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C32:E32"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C50:E50"/>
@@ -3385,16 +3540,8 @@
     <mergeCell ref="C58:E58"/>
     <mergeCell ref="C59:E59"/>
     <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="C135:D135"/>
-    <mergeCell ref="C161:D161"/>
-    <mergeCell ref="C154:D154"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C168:D168"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>